<commit_message>
Updating the sheet pool names in the bmo small business spreadsheet data.
</commit_message>
<xml_diff>
--- a/app/data/pools/bmo_sb.xlsx
+++ b/app/data/pools/bmo_sb.xlsx
@@ -5,28 +5,28 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="BMO_SB_MASTER" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="BMO_SB" sheetId="2" state="hidden" r:id="rId3"/>
-    <sheet name="SB Pool 1 - HVAC" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="SB Pool 2 - Plumbing" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="SB Pool 3 - ElevM" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="SB Pool 4 - ElecM" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="SB Pool 5 - Jan" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="SB Pool 6 - LndScp" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="SB Pool 7 - FrSysM" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="SB Pool 8 - FrSupr" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="SB Pool 9 - Roof" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="SB Pool 10 - BldMgmt" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="SB Pool 11 - Archt" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="SB Pool 12 - CommS" sheetId="14" state="visible" r:id="rId15"/>
-    <sheet name="SB Pool 13 - ElevIns" sheetId="15" state="visible" r:id="rId16"/>
-    <sheet name="SB Pool 14 - FacMgmt" sheetId="16" state="visible" r:id="rId17"/>
-    <sheet name="SB Pool 15 - Pest" sheetId="17" state="visible" r:id="rId18"/>
-    <sheet name="SB Pool 16 - WstMgmt" sheetId="18" state="visible" r:id="rId19"/>
-    <sheet name="SB Pool 17 - Cemetary" sheetId="19" state="visible" r:id="rId20"/>
+    <sheet name="SB Pool (1) - HVAC" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="SB Pool (2) - Plumbing" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="SB Pool (3) - ElevM" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="SB Pool (4) - ElecM" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="SB Pool (5) - Jan" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="SB Pool (6) - LndScp" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="SB Pool (7) - FrSysM" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="SB Pool (8) - FrSupr" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="SB Pool (9) - Roof" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="SB Pool (10) - BldMgmt" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="SB Pool (11) - Archt" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="SB Pool (12) - CommS" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="SB Pool (13) - ElevIns" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="SB Pool (14) - FacMgmt" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="SB Pool (15) - Pest" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="SB Pool (16) - WstMgmt" sheetId="18" state="visible" r:id="rId19"/>
+    <sheet name="SB Pool (17) - Cemetary" sheetId="19" state="visible" r:id="rId20"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1569,7 +1569,7 @@
     <numFmt numFmtId="166" formatCode="@"/>
     <numFmt numFmtId="167" formatCode="M/D/YYYY"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1591,13 +1591,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1812,7 +1805,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1836,10 +1829,6 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="61">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1850,51 +1839,47 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1902,175 +1887,179 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="6" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2078,23 +2067,22 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -2177,7 +2165,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.17"/>
@@ -7002,7 +6990,7 @@
   </sheetPr>
   <dimension ref="A1:Y45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -24873,7 +24861,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.17"/>
@@ -35151,7 +35139,7 @@
   </sheetPr>
   <dimension ref="A1:Y49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -35167,7 +35155,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="28.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="24.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="24.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="3.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="8.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="4.63"/>

</xml_diff>